<commit_message>
Hopefully the last graphs I have to make
</commit_message>
<xml_diff>
--- a/Regression Analysis/Final project/Summary.xlsx
+++ b/Regression Analysis/Final project/Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Prokopius\Documents\FALCON HD\GitHub\Reproducible-Science\Sparkle Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Prokopius\Documents\FALCON HD\GitHub\Reproducible-Science\Regression Analysis\Final project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAAB683-2E9F-4B56-AB9F-940C6E0CE996}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EB86DC-8E23-48D8-ABB0-621805F327D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{9EB31290-BA9C-42D0-A1EE-93E261E87E94}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="3" xr2:uid="{9EB31290-BA9C-42D0-A1EE-93E261E87E94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sig relationships" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="48">
   <si>
     <t>Model Type</t>
   </si>
@@ -160,13 +160,31 @@
   </si>
   <si>
     <t>Bracgycentridae-Noninear</t>
+  </si>
+  <si>
+    <t>R squared value</t>
+  </si>
+  <si>
+    <t>Taxa level</t>
+  </si>
+  <si>
+    <t>Order-Trichoptera</t>
+  </si>
+  <si>
+    <t>Family-Hydropsychidae</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>Natural log transformed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +205,12 @@
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -219,6 +243,7 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,7 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936A05EB-14BD-4F22-AD93-1AB971C911F3}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F21"/>
     </sheetView>
   </sheetViews>
@@ -1923,7 +1948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC760289-ACC9-480F-89AC-D47A11D5C391}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16:F31"/>
     </sheetView>
   </sheetViews>
@@ -2655,551 +2680,659 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351B3ABF-0CA0-4D5A-8CE2-902A803FBD65}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>478.8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1">
         <v>0.65690000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
+        <v>878</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1250</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.77839999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1">
         <v>388</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="G4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1">
         <v>0.60809999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E5" s="1">
+        <v>888.8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.78049999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1">
         <v>392.1</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1">
+      <c r="G6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="1">
         <v>0.64910000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E7" s="1">
+        <v>904.9</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.81020000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1">
         <v>367.1</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="G8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="1">
         <v>0.63390000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1">
-        <v>14.44</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1.9499999999999999E-3</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.50780000000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1">
-        <v>9.1300000000000008</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="1">
-        <v>9.1500000000000001E-3</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.3947</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="1">
-        <v>38.659999999999997</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.6946</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1">
-        <v>10.62</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="1">
-        <v>4.62E-3</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.3846</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <v>870.7</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.80420000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="1">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1">
         <v>808.7</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1">
         <v>0.78010000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="1">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2073</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.90090000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1">
         <v>520.70000000000005</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="1">
+      <c r="G12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.69550000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="1">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1236</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.84430000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="1">
         <v>713.4</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="1">
+      <c r="G14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="1">
         <v>0.79579999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="1">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1911</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.91259999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1">
         <v>450.8</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="1">
+      <c r="G16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="1">
         <v>0.71130000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="1">
-        <v>9.18</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1.0500000000000001E-2</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0.43340000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="1">
-        <v>12.13</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="1">
-        <v>4.5199999999999997E-3</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0.50270000000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="1">
-        <v>169.5</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0.92879999999999996</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="1">
-        <v>29.23</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1.198E-4</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0.69220000000000004</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1180</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.86570000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="1">
-        <v>15.34</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="1">
-        <v>2.4099999999999998E-3</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0.58230000000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="1">
+        <v>113.7</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.5474</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="1">
-        <v>8.468</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1.4200000000000001E-2</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0.435</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="1">
+        <v>457.1</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.82940000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="1">
-        <v>113.7</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1">
+        <v>98.74</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0.5474</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.51229999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="1">
-        <v>98.74</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="1">
+        <v>379.9</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0.51229999999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.80159999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>112.6</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="1">
+      <c r="G22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="1">
         <v>0.56710000000000005</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="1">
         <v>89.06</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="1">
+      <c r="G24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="1">
         <v>0.50870000000000004</v>
       </c>
     </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>